<commit_message>
docs: update README with usage instructions and refresh benchmarks
- Added Installation guide (Ollama setup, pip install).
- Added Usage examples for `classifier.py`, `sample_generator.py`, and `sample_analyzer.py`.
- Documented Sample Generation and Analyzer features.
- Added License information.
- Updated benchmark Excel files.
</commit_message>
<xml_diff>
--- a/data/benchmarks/dataset_comparison.xlsx
+++ b/data/benchmarks/dataset_comparison.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
-    <t xml:space="preserve">Tecniche di Prompting</t>
+    <t xml:space="preserve">Prompting Method</t>
   </si>
   <si>
     <t>Zero-Shot</t>
@@ -189,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -203,13 +203,7 @@
     <xf fontId="0" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf fontId="1" fillId="6" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="7" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="7" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -733,7 +727,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="G15" zoomScale="74" workbookViewId="0">
+    <sheetView topLeftCell="E15" zoomScale="74" workbookViewId="0">
       <selection activeCell="Q6" activeCellId="0" sqref="Q6"/>
     </sheetView>
   </sheetViews>
@@ -1133,201 +1127,201 @@
       <c r="M15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N15" s="5" t="s">
+      <c r="N15" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" ht="30.600000000000001" customHeight="1"/>
     <row r="18" ht="30" customHeight="1"/>
     <row r="19" ht="30" customHeight="1">
-      <c r="A19" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="7" t="s">
+      <c r="A19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E19" s="7" t="s">
+      <c r="D19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G19" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="H19" s="7" t="s">
+      <c r="G19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="K19" s="7" t="s">
+      <c r="J19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K19" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M19" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="N19" s="7" t="s">
+      <c r="M19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="N19" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="20" ht="31.800000000000001" customHeight="1">
-      <c r="A20" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" s="7" t="s">
+      <c r="A20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="7" t="s">
+      <c r="D20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H20" s="7" t="s">
+      <c r="G20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J20" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="K20" s="7" t="s">
+      <c r="J20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K20" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="M20" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="N20" s="7" t="s">
+      <c r="M20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N20" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" ht="29.399999999999999" customHeight="1">
-      <c r="A21" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="7">
-        <v>3000</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="7">
-        <v>3000</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21" s="7">
-        <v>3000</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="K21" s="7">
-        <v>3000</v>
-      </c>
-      <c r="M21" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="N21" s="7">
+      <c r="A21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="6">
+        <v>3000</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="6">
+        <v>3000</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="6">
+        <v>3000</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K21" s="6">
+        <v>3000</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N21" s="6">
         <v>3000</v>
       </c>
     </row>
     <row r="22" ht="30.600000000000001" customHeight="1">
-      <c r="A22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="7">
+      <c r="A22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="6">
         <v>2004</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="7">
+      <c r="D22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="6">
         <v>2410</v>
       </c>
-      <c r="G22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H22" s="7">
+      <c r="G22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="6">
         <v>2332</v>
       </c>
-      <c r="J22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="K22" s="7">
+      <c r="J22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" s="6">
         <v>2119</v>
       </c>
-      <c r="M22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="N22" s="7">
+      <c r="M22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="N22" s="6">
         <v>2323</v>
       </c>
     </row>
     <row r="23" ht="28.199999999999999" customHeight="1">
-      <c r="A23" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="7">
+      <c r="A23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="6">
         <v>996</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="7">
+      <c r="D23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="6">
         <v>590</v>
       </c>
-      <c r="G23" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23" s="7">
+      <c r="G23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="6">
         <v>668</v>
       </c>
-      <c r="J23" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K23" s="7">
+      <c r="J23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K23" s="6">
         <v>881</v>
       </c>
-      <c r="M23" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="N23" s="7">
+      <c r="M23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N23" s="6">
         <v>677</v>
       </c>
     </row>
     <row r="24" ht="28.199999999999999" customHeight="1">
-      <c r="A24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="7" t="s">
+      <c r="A24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="7" t="s">
+      <c r="D24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H24" s="7" t="s">
+      <c r="G24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K24" s="7" t="s">
+      <c r="J24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K24" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="M24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N24" s="8" t="s">
+      <c r="M24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N24" s="6" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>